<commit_message>
Cambiado el doParse y test2.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/test2.xlsx
+++ b/src/test/resources/test2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Oriol\Documents\aswGrupo\citizensLoader_i3b\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acoto\OneDrive\TERCERO\Segundo Cuatrimestre\Arquitectura del Software\Deliverable-1\Loader_i3a\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,51 +30,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>90500084Y</t>
-  </si>
-  <si>
-    <t>C/ Federico García Lorca 2</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
     <t>juan@example.com</t>
   </si>
   <si>
-    <t>Dirección postal</t>
-  </si>
-  <si>
-    <t>NIF</t>
-  </si>
-  <si>
-    <t>pollingStation</t>
+    <t>Juan Torres Pardo</t>
+  </si>
+  <si>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>40.5N30.99W</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Tipo</t>
   </si>
 </sst>
 </file>
@@ -121,8 +100,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -404,74 +383,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1">
-        <v>31330</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
+      <c r="D2">
+        <v>123</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
     </row>

</xml_diff>